<commit_message>
cleaned dependency up a bit re-enacted the hard coded other exclusion allowed excluded sessions to run
</commit_message>
<xml_diff>
--- a/Projects/RINIELSENUS/Data/Template_2019 SPT Baseline_v1.01.xlsx
+++ b/Projects/RINIELSENUS/Data/Template_2019 SPT Baseline_v1.01.xlsx
@@ -56,6 +56,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hierarchy!$A$1:$L$120</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hierarchy!$A$1:$L$120</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hierarchy!$A$1:$L$120</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hierarchy!$A$1:$L$120</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
@@ -71,14 +72,15 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
@@ -86,6 +88,7 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
@@ -101,6 +104,7 @@
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
@@ -116,6 +120,7 @@
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
@@ -131,6 +136,7 @@
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
+    <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -7745,11 +7751,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.5182186234818"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
@@ -7819,22 +7825,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="95.2267206477733"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="96.085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="53.668016194332"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="33.4210526315789"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.3886639676113"/>
@@ -8223,17 +8229,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="43.0607287449393"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="43.4898785425101"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.78542510121457"/>
   </cols>
@@ -8357,14 +8363,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="77.7692307692308"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.412955465587"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.78542510121457"/>
   </cols>
@@ -8729,12 +8735,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.3036437246964"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -8828,11 +8834,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
@@ -8881,18 +8887,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.6234817813765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.3765182186235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="123.295546558704"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="124.473684210526"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.78542510121457"/>
   </cols>
@@ -8962,12 +8968,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.2712550607287"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
@@ -9019,9 +9025,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -9104,9 +9110,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.8785425101215"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.412955465587"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
@@ -9180,11 +9186,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0283400809717"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4574898785425"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -20421,16 +20427,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.3076923076923"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.9473684210526"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.0242914979757"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.78542510121457"/>
   </cols>
@@ -24506,12 +24512,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="58" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="58" width="44.668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="58" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="58" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="58" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="58" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="58" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="58" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="58" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="58" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="58" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="58" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="58" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="58" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -24848,23 +24854,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="74.6599190283401"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="75.3036437246964"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="9" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="9" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="9" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="9" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="9" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="9" width="47.7732793522267"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="9" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="9" width="48.2024291497976"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="9" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="9" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="9" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -24975,21 +24981,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.8866396761134"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="59.3441295546559"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="53.668016194332"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.1012145748988"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="59.8785425101215"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -25259,13 +25265,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="77.3400809716599"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="77.9838056680162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
   </cols>
@@ -25538,14 +25544,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.5141700404858"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="88.3724696356275"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
   </cols>
@@ -25717,12 +25723,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="9" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="35.0283400809717"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="35.2429149797571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="9" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -40131,28 +40137,28 @@
   </sheetPr>
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.6963562753036"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.78542510121457"/>
@@ -40230,6 +40236,9 @@
       <c r="I2" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R2" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40253,6 +40262,9 @@
       <c r="I3" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M3" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R3" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40276,6 +40288,9 @@
       <c r="I4" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M4" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R4" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40283,7 +40298,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -40299,6 +40314,9 @@
       <c r="I5" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M5" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R5" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40306,7 +40324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -40322,6 +40340,9 @@
       <c r="I6" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M6" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R6" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40329,7 +40350,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
@@ -40348,6 +40369,9 @@
       <c r="I7" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M7" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R7" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40355,7 +40379,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -40374,6 +40398,9 @@
       <c r="I8" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M8" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R8" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40381,7 +40408,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -40394,6 +40421,9 @@
       <c r="F9" s="0" t="s">
         <v>191</v>
       </c>
+      <c r="M9" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R9" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40401,7 +40431,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>71</v>
       </c>
@@ -40417,6 +40447,9 @@
       <c r="G10" s="0" t="s">
         <v>700</v>
       </c>
+      <c r="M10" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R10" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40424,7 +40457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>71</v>
       </c>
@@ -40440,6 +40473,9 @@
       <c r="G11" s="0" t="s">
         <v>701</v>
       </c>
+      <c r="M11" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R11" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40447,7 +40483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>71</v>
       </c>
@@ -40463,6 +40499,9 @@
       <c r="G12" s="0" t="s">
         <v>702</v>
       </c>
+      <c r="M12" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R12" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40470,7 +40509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>71</v>
       </c>
@@ -40486,6 +40525,9 @@
       <c r="I13" s="0" t="s">
         <v>213</v>
       </c>
+      <c r="M13" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R13" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40493,7 +40535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>71</v>
       </c>
@@ -40512,6 +40554,9 @@
       <c r="L14" s="0" t="s">
         <v>703</v>
       </c>
+      <c r="M14" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R14" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40519,7 +40564,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
         <v>71</v>
       </c>
@@ -40538,6 +40583,9 @@
       <c r="L15" s="0" t="s">
         <v>704</v>
       </c>
+      <c r="M15" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R15" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40545,7 +40593,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>71</v>
       </c>
@@ -40564,6 +40612,9 @@
       <c r="L16" s="0" t="s">
         <v>705</v>
       </c>
+      <c r="M16" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R16" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40571,7 +40622,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>71</v>
       </c>
@@ -40587,6 +40638,9 @@
       <c r="I17" s="0" t="s">
         <v>214</v>
       </c>
+      <c r="M17" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R17" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40594,7 +40648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
         <v>71</v>
       </c>
@@ -40613,6 +40667,9 @@
       <c r="L18" s="63" t="s">
         <v>703</v>
       </c>
+      <c r="M18" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R18" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40620,7 +40677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>71</v>
       </c>
@@ -40639,6 +40696,9 @@
       <c r="L19" s="63" t="s">
         <v>704</v>
       </c>
+      <c r="M19" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R19" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40646,7 +40706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
         <v>71</v>
       </c>
@@ -40665,6 +40725,9 @@
       <c r="L20" s="63" t="s">
         <v>706</v>
       </c>
+      <c r="M20" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R20" s="79" t="n">
         <v>0.75</v>
       </c>
@@ -40672,7 +40735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
         <v>105</v>
       </c>
@@ -40688,6 +40751,9 @@
       <c r="I21" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M21" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q21" s="0" t="s">
         <v>224</v>
       </c>
@@ -40698,7 +40764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>105</v>
       </c>
@@ -40714,6 +40780,9 @@
       <c r="I22" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M22" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q22" s="0" t="s">
         <v>224</v>
       </c>
@@ -40724,7 +40793,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>105</v>
       </c>
@@ -40743,6 +40812,9 @@
       <c r="J23" s="82" t="s">
         <v>707</v>
       </c>
+      <c r="M23" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q23" s="0" t="s">
         <v>224</v>
       </c>
@@ -40753,7 +40825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>105</v>
       </c>
@@ -40772,6 +40844,9 @@
       <c r="J24" s="82" t="s">
         <v>708</v>
       </c>
+      <c r="M24" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q24" s="0" t="s">
         <v>224</v>
       </c>
@@ -40782,7 +40857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>105</v>
       </c>
@@ -40801,6 +40876,9 @@
       <c r="J25" s="0" t="s">
         <v>709</v>
       </c>
+      <c r="M25" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q25" s="0" t="s">
         <v>224</v>
       </c>
@@ -40811,7 +40889,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
         <v>105</v>
       </c>
@@ -40830,6 +40908,9 @@
       <c r="J26" s="82" t="s">
         <v>710</v>
       </c>
+      <c r="M26" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q26" s="0" t="s">
         <v>224</v>
       </c>
@@ -40840,7 +40921,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>105</v>
       </c>
@@ -40859,6 +40940,9 @@
       <c r="J27" s="82" t="s">
         <v>707</v>
       </c>
+      <c r="M27" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q27" s="0" t="s">
         <v>224</v>
       </c>
@@ -40869,7 +40953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>105</v>
       </c>
@@ -40888,6 +40972,9 @@
       <c r="J28" s="82" t="s">
         <v>710</v>
       </c>
+      <c r="M28" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q28" s="0" t="s">
         <v>224</v>
       </c>
@@ -40898,7 +40985,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
         <v>105</v>
       </c>
@@ -40917,6 +41004,9 @@
       <c r="J29" s="82" t="s">
         <v>708</v>
       </c>
+      <c r="M29" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q29" s="0" t="s">
         <v>224</v>
       </c>
@@ -40927,7 +41017,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
         <v>105</v>
       </c>
@@ -40946,6 +41036,9 @@
       <c r="J30" s="82" t="s">
         <v>707</v>
       </c>
+      <c r="M30" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q30" s="0" t="s">
         <v>224</v>
       </c>
@@ -40956,7 +41049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
         <v>105</v>
       </c>
@@ -40975,6 +41068,9 @@
       <c r="J31" s="82" t="s">
         <v>708</v>
       </c>
+      <c r="M31" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q31" s="0" t="s">
         <v>224</v>
       </c>
@@ -40985,7 +41081,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
         <v>105</v>
       </c>
@@ -41004,6 +41100,9 @@
       <c r="J32" s="0" t="s">
         <v>709</v>
       </c>
+      <c r="M32" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q32" s="0" t="s">
         <v>224</v>
       </c>
@@ -41014,7 +41113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
         <v>105</v>
       </c>
@@ -41033,6 +41132,9 @@
       <c r="J33" s="82" t="s">
         <v>710</v>
       </c>
+      <c r="M33" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q33" s="0" t="s">
         <v>224</v>
       </c>
@@ -41043,7 +41145,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
         <v>105</v>
       </c>
@@ -41059,6 +41161,9 @@
       <c r="I34" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M34" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q34" s="0" t="s">
         <v>224</v>
       </c>
@@ -41069,7 +41174,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
         <v>105</v>
       </c>
@@ -41085,6 +41190,9 @@
       <c r="I35" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M35" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q35" s="0" t="s">
         <v>224</v>
       </c>
@@ -41095,7 +41203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
         <v>105</v>
       </c>
@@ -41111,6 +41219,9 @@
       <c r="I36" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M36" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q36" s="0" t="s">
         <v>224</v>
       </c>
@@ -41121,7 +41232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
         <v>105</v>
       </c>
@@ -41137,6 +41248,9 @@
       <c r="I37" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M37" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q37" s="0" t="s">
         <v>224</v>
       </c>
@@ -41147,7 +41261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
         <v>105</v>
       </c>
@@ -41163,6 +41277,9 @@
       <c r="I38" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M38" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q38" s="0" t="s">
         <v>224</v>
       </c>
@@ -41173,7 +41290,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
         <v>105</v>
       </c>
@@ -41189,6 +41306,9 @@
       <c r="I39" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M39" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q39" s="0" t="s">
         <v>224</v>
       </c>
@@ -41199,7 +41319,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
         <v>105</v>
       </c>
@@ -41215,6 +41335,9 @@
       <c r="I40" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M40" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q40" s="0" t="s">
         <v>224</v>
       </c>
@@ -41225,7 +41348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
         <v>105</v>
       </c>
@@ -41241,6 +41364,9 @@
       <c r="I41" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="M41" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q41" s="0" t="s">
         <v>224</v>
       </c>
@@ -41251,7 +41377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
         <v>145</v>
       </c>
@@ -41264,6 +41390,9 @@
       <c r="F42" s="0" t="s">
         <v>196</v>
       </c>
+      <c r="M42" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q42" s="0" t="s">
         <v>226</v>
       </c>
@@ -41274,7 +41403,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
         <v>145</v>
       </c>
@@ -41290,6 +41419,9 @@
       <c r="G43" s="0" t="s">
         <v>715</v>
       </c>
+      <c r="M43" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q43" s="0" t="s">
         <v>226</v>
       </c>
@@ -41300,7 +41432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
         <v>145</v>
       </c>
@@ -41316,6 +41448,9 @@
       <c r="G44" s="0" t="s">
         <v>716</v>
       </c>
+      <c r="M44" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q44" s="0" t="s">
         <v>226</v>
       </c>
@@ -41326,7 +41461,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
         <v>145</v>
       </c>
@@ -41342,6 +41477,9 @@
       <c r="G45" s="0" t="s">
         <v>717</v>
       </c>
+      <c r="M45" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q45" s="0" t="s">
         <v>226</v>
       </c>
@@ -41352,7 +41490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
         <v>145</v>
       </c>
@@ -41368,6 +41506,9 @@
       <c r="G46" s="0" t="s">
         <v>225</v>
       </c>
+      <c r="M46" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q46" s="0" t="s">
         <v>226</v>
       </c>
@@ -41378,7 +41519,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
         <v>145</v>
       </c>
@@ -41394,6 +41535,9 @@
       <c r="G47" s="0" t="s">
         <v>715</v>
       </c>
+      <c r="M47" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q47" s="0" t="s">
         <v>226</v>
       </c>
@@ -41404,7 +41548,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
         <v>145</v>
       </c>
@@ -41420,6 +41564,9 @@
       <c r="G48" s="0" t="s">
         <v>716</v>
       </c>
+      <c r="M48" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q48" s="0" t="s">
         <v>226</v>
       </c>
@@ -41430,7 +41577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
         <v>145</v>
       </c>
@@ -41446,6 +41593,9 @@
       <c r="G49" s="0" t="s">
         <v>717</v>
       </c>
+      <c r="M49" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q49" s="0" t="s">
         <v>226</v>
       </c>
@@ -41456,7 +41606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
         <v>145</v>
       </c>
@@ -41472,6 +41622,9 @@
       <c r="G50" s="0" t="s">
         <v>225</v>
       </c>
+      <c r="M50" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q50" s="0" t="s">
         <v>226</v>
       </c>
@@ -41482,7 +41635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
         <v>145</v>
       </c>
@@ -41501,6 +41654,9 @@
       <c r="J51" s="0" t="s">
         <v>719</v>
       </c>
+      <c r="M51" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q51" s="0" t="s">
         <v>226</v>
       </c>
@@ -41511,7 +41667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
         <v>145</v>
       </c>
@@ -41530,6 +41686,9 @@
       <c r="J52" s="0" t="s">
         <v>720</v>
       </c>
+      <c r="M52" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q52" s="0" t="s">
         <v>226</v>
       </c>
@@ -41540,7 +41699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
         <v>145</v>
       </c>
@@ -41559,6 +41718,9 @@
       <c r="J53" s="0" t="s">
         <v>721</v>
       </c>
+      <c r="M53" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q53" s="0" t="s">
         <v>226</v>
       </c>
@@ -41569,7 +41731,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
         <v>145</v>
       </c>
@@ -41588,6 +41750,9 @@
       <c r="J54" s="0" t="s">
         <v>722</v>
       </c>
+      <c r="M54" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q54" s="0" t="s">
         <v>226</v>
       </c>
@@ -41598,7 +41763,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
         <v>145</v>
       </c>
@@ -41617,6 +41782,9 @@
       <c r="J55" s="0" t="s">
         <v>723</v>
       </c>
+      <c r="M55" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q55" s="0" t="s">
         <v>226</v>
       </c>
@@ -41627,7 +41795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
         <v>145</v>
       </c>
@@ -41646,6 +41814,9 @@
       <c r="J56" s="0" t="s">
         <v>724</v>
       </c>
+      <c r="M56" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q56" s="0" t="s">
         <v>226</v>
       </c>
@@ -41656,7 +41827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
         <v>105</v>
       </c>
@@ -41671,6 +41842,9 @@
       </c>
       <c r="I57" s="0" t="s">
         <v>221</v>
+      </c>
+      <c r="M57" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="N57" s="0" t="s">
         <v>178</v>

</xml_diff>

<commit_message>
excluded sessions now added back in with template change for preferred range
</commit_message>
<xml_diff>
--- a/Projects/RINIELSENUS/Data/Template_2019 SPT Baseline_v1.01.xlsx
+++ b/Projects/RINIELSENUS/Data/Template_2019 SPT Baseline_v1.01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="change log" sheetId="1" state="visible" r:id="rId2"/>
@@ -57,6 +57,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hierarchy!$A$1:$L$120</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hierarchy!$A$1:$L$120</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hierarchy!$A$1:$L$120</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hierarchy!$A$1:$L$120</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
@@ -73,15 +74,16 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">NBIL!$A$1:$S$894</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$57</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
@@ -89,6 +91,7 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Block!$A$1:$R$56</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
@@ -105,6 +108,7 @@
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Adjacency!$A$1:$U$1</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
@@ -121,6 +125,7 @@
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Linear fair share'!$A$1:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
@@ -137,6 +142,7 @@
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
+    <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Segment_LU!$C$2:$E$1005</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -7751,11 +7757,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.5951417004049"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="73.1619433198381"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
@@ -7825,22 +7831,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="96.085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0283400809717"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="96.9433198380567"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.2429149797571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="54.0931174089069"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="33.7408906882591"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.3886639676113"/>
@@ -8229,17 +8235,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="43.8097165991903"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.78542510121457"/>
   </cols>
@@ -8363,14 +8369,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.78542510121457"/>
   </cols>
@@ -8735,12 +8741,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.0526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -8834,11 +8840,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
@@ -8887,18 +8893,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.3765182186235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.0161943319838"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="124.473684210526"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="125.542510121458"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.78542510121457"/>
   </cols>
@@ -8968,12 +8974,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.2712550607287"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.8056680161943"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
@@ -9019,15 +9025,15 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -9061,7 +9067,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="99" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9110,9 +9116,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
@@ -9186,11 +9192,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3481781376518"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -20419,24 +20425,24 @@
   </sheetPr>
   <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D82" activeCellId="0" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.9473684210526"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.5910931174089"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.4493927125506"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.78542510121457"/>
   </cols>
@@ -24512,12 +24518,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="58" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="58" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="58" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="58" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="58" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="58" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="58" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="58" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="58" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="58" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="58" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="58" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="58" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="58" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -24854,23 +24860,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="75.3036437246964"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="75.9473684210526"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="9" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="9" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="9" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="9" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="9" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="9" width="48.2024291497976"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="9" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="9" width="48.6315789473684"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="9" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="9" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="9" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -24981,21 +24987,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.1619433198381"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.8016194331984"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="59.8785425101215"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="54.0931174089069"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.4210526315789"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -25265,13 +25271,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="77.9838056680162"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.6234817813765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
   </cols>
@@ -25544,14 +25550,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="88.3724696356275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="89.1214574898785"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
   </cols>
@@ -25723,12 +25729,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="9" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="35.2429149797571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="9" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -40137,28 +40143,28 @@
   </sheetPr>
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.3400809716599"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.4574898785425"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.78542510121457"/>

</xml_diff>